<commit_message>
Resolved issue with exit button always taking to motorcycle menu
</commit_message>
<xml_diff>
--- a/MindaButtonEvntFnCalls.xlsx
+++ b/MindaButtonEvntFnCalls.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d410da21e816d252/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ReyoctoRepo\KTMButtonLogic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{346989B4-3992-4FE8-8D1A-6BF8F6E454EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C043944-84A4-4900-8091-54122B9D461F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DD19BDDD-8E1B-4297-BF4B-B3726D1FA863}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="169">
   <si>
     <t>Action Event</t>
   </si>
@@ -516,6 +516,33 @@
   </si>
   <si>
     <t>Sno</t>
+  </si>
+  <si>
+    <t>POPUP_INCALL_INSTRUCTION</t>
+  </si>
+  <si>
+    <t>BLU_FnIncomingCallAnswer()</t>
+  </si>
+  <si>
+    <t>EXIT</t>
+  </si>
+  <si>
+    <t>BLU_FnIncomingCallReject()</t>
+  </si>
+  <si>
+    <t>ACTIVE_CALL</t>
+  </si>
+  <si>
+    <t>BLU_FnCallVolDec()</t>
+  </si>
+  <si>
+    <t>BLU_FnCallVolInc()</t>
+  </si>
+  <si>
+    <t>BLU_FnActvCallEXIT()</t>
+  </si>
+  <si>
+    <t>BLU_FnActvCallSET()</t>
   </si>
 </sst>
 </file>
@@ -693,34 +720,6 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -797,13 +796,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -816,6 +808,41 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -832,22 +859,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20F3215A-34DA-46B1-806F-A2A772BDAE46}" name="Table1" displayName="Table1" ref="A1:D150" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
-  <autoFilter ref="A1:D150" xr:uid="{20F3215A-34DA-46B1-806F-A2A772BDAE46}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20F3215A-34DA-46B1-806F-A2A772BDAE46}" name="Table1" displayName="Table1" ref="A1:D157" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="A1:D157" xr:uid="{20F3215A-34DA-46B1-806F-A2A772BDAE46}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D8B4643F-5EBC-4FFB-A84B-6FC2A8482A8F}" name="Sno" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{145C72FF-D314-4190-B5DC-91F4208D13EB}" name="Screen" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{BB351AB9-CF4B-4A66-A4B0-12E4B7D74926}" name="Action Event" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{ED9B5C58-5D3D-487B-B6CD-38C10DE38570}" name="Function Call " dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{D8B4643F-5EBC-4FFB-A84B-6FC2A8482A8F}" name="Sno" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{145C72FF-D314-4190-B5DC-91F4208D13EB}" name="Screen" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{BB351AB9-CF4B-4A66-A4B0-12E4B7D74926}" name="Action Event" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{ED9B5C58-5D3D-487B-B6CD-38C10DE38570}" name="Function Call " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -885,7 +912,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -991,7 +1018,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1133,7 +1160,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1141,10 +1168,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22FCE55C-9D52-4F04-BCD1-AFEB7F180101}">
-  <dimension ref="A1:D150"/>
+  <dimension ref="A1:D157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="B151" sqref="B151:D156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3253,6 +3280,96 @@
         <v>153</v>
       </c>
     </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="7">
+        <v>150</v>
+      </c>
+      <c r="B151" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C151" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D151" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="7">
+        <v>151</v>
+      </c>
+      <c r="B152" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C152" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D152" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="7">
+        <v>152</v>
+      </c>
+      <c r="B153" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C153" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D153" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="7">
+        <v>153</v>
+      </c>
+      <c r="B154" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C154" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D154" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="7">
+        <v>154</v>
+      </c>
+      <c r="B155" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C155" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D155" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="7">
+        <v>155</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C156" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D156" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="7"/>
+      <c r="B157" s="8"/>
+      <c r="C157" s="8"/>
+      <c r="D157" s="9"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>